<commit_message>
Add BobEvans and McDonalds data
</commit_message>
<xml_diff>
--- a/Datas/DatabaseList.xlsx
+++ b/Datas/DatabaseList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven Lu\Desktop\Current Project\ISPTerm\Datas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven Lu\Desktop\ISPTerm\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795AA569-AE85-4537-8E28-C231B4E2C3D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14B4080-1817-4AFD-B562-F37DD83F0D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{86EB7131-618B-4289-935E-0A00109B9DA8}"/>
+    <workbookView xWindow="38280" yWindow="-7155" windowWidth="16440" windowHeight="28320" xr2:uid="{86EB7131-618B-4289-935E-0A00109B9DA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="354">
   <si>
     <t>calories</t>
   </si>
@@ -501,6 +501,660 @@
   </si>
   <si>
     <t>TEX-MEX SHRIMP BOWL</t>
+  </si>
+  <si>
+    <t>BobEvan's</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Farmhand Biscuit Sandwich Platter
+</t>
+  </si>
+  <si>
+    <t>13.29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Original Farmer's Choice
+</t>
+  </si>
+  <si>
+    <t>1070</t>
+  </si>
+  <si>
+    <t>11.29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Double Meat Farmer's Choice
+</t>
+  </si>
+  <si>
+    <t>13.89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Banana Berry Farmer
+</t>
+  </si>
+  <si>
+    <t>1270</t>
+  </si>
+  <si>
+    <t>13.19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rise &amp; Shine
+</t>
+  </si>
+  <si>
+    <t>870</t>
+  </si>
+  <si>
+    <t>10.19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homestead Farmer
+</t>
+  </si>
+  <si>
+    <t>930</t>
+  </si>
+  <si>
+    <t>12.29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Whole Hog
+</t>
+  </si>
+  <si>
+    <t>1800</t>
+  </si>
+  <si>
+    <t>14.29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Everything Breakfast
+</t>
+  </si>
+  <si>
+    <t>1130</t>
+  </si>
+  <si>
+    <t>12.69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Big Egg Breakfast
+</t>
+  </si>
+  <si>
+    <t>690</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country-Fried Steak &amp; Farm-Fresh Eggs
+</t>
+  </si>
+  <si>
+    <t>1310</t>
+  </si>
+  <si>
+    <t>11.89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sirloin Steak* &amp; Farm-Fresh Eggs
+</t>
+  </si>
+  <si>
+    <t>13.99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country Biscuit
+</t>
+  </si>
+  <si>
+    <t>7.79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blue Ribbon Bacon
+</t>
+  </si>
+  <si>
+    <t>390</t>
+  </si>
+  <si>
+    <t>4.99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cinna-Biscuits
+</t>
+  </si>
+  <si>
+    <t>700</t>
+  </si>
+  <si>
+    <t>3.99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southwest Avocado Omelet
+</t>
+  </si>
+  <si>
+    <t>750</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Three Meat &amp; Cheese Omelet
+</t>
+  </si>
+  <si>
+    <t>1820</t>
+  </si>
+  <si>
+    <t>12.49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Build Your Own Omelet
+</t>
+  </si>
+  <si>
+    <t>11.49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western Omelet
+</t>
+  </si>
+  <si>
+    <t>11.69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sunshine Skillet
+</t>
+  </si>
+  <si>
+    <t>1180</t>
+  </si>
+  <si>
+    <t>10.99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Double Cheese Pot Roast Dip
+</t>
+  </si>
+  <si>
+    <t>12.09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Farmhouse Hand-Breaded Fried Chicken Sandwich
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All American BLT
+</t>
+  </si>
+  <si>
+    <t>10.09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bacon Cheeseburger
+</t>
+  </si>
+  <si>
+    <t>840</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steakhouse Burger
+</t>
+  </si>
+  <si>
+    <t>12.79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rise &amp; Shine Burger
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cheeseburger
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Farmhouse Grilled Chicken Sandwich
+</t>
+  </si>
+  <si>
+    <t>McDonald's</t>
+  </si>
+  <si>
+    <t>Crispy Chicken Sandwich (Spicy Deluxe)</t>
+  </si>
+  <si>
+    <t>530</t>
+  </si>
+  <si>
+    <t>6.99</t>
+  </si>
+  <si>
+    <t>Crispy Chicken Sandwich</t>
+  </si>
+  <si>
+    <t>470</t>
+  </si>
+  <si>
+    <t>6.19</t>
+  </si>
+  <si>
+    <t>Chicken Sandwich (Spicy Crispy)</t>
+  </si>
+  <si>
+    <t>Chicken Sandwich (Deluxe Crispy)</t>
+  </si>
+  <si>
+    <t>Chicken McNuggets</t>
+  </si>
+  <si>
+    <t>170</t>
+  </si>
+  <si>
+    <t>McChicken</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>Filet O Fish</t>
+  </si>
+  <si>
+    <t>6.69</t>
+  </si>
+  <si>
+    <t>Big Mac Combo Meal</t>
+  </si>
+  <si>
+    <t>Cheeseburger Combo Meal</t>
+  </si>
+  <si>
+    <t>830</t>
+  </si>
+  <si>
+    <t>Double Quarter Pounder with Cheese Meal</t>
+  </si>
+  <si>
+    <t>14.39</t>
+  </si>
+  <si>
+    <t>Combo Crispy Chicken Sandwich Meal</t>
+  </si>
+  <si>
+    <t>990</t>
+  </si>
+  <si>
+    <t>12.97</t>
+  </si>
+  <si>
+    <t>Combo Chicken Sandwich (Spicy &amp; Crispy)</t>
+  </si>
+  <si>
+    <t>13.81</t>
+  </si>
+  <si>
+    <t>Combo Chicken Sandwich (Deluxe Crispy)</t>
+  </si>
+  <si>
+    <t>Chicken McNuggets â€“ 10 Count</t>
+  </si>
+  <si>
+    <t>Egg McMuffin</t>
+  </si>
+  <si>
+    <t>450</t>
+  </si>
+  <si>
+    <t>2.79</t>
+  </si>
+  <si>
+    <t>Sausage McMuffin (with Egg Meal)</t>
+  </si>
+  <si>
+    <t>4.19</t>
+  </si>
+  <si>
+    <t>Sausage Biscuit included Egg Meal</t>
+  </si>
+  <si>
+    <t>670</t>
+  </si>
+  <si>
+    <t>Bacon, Egg &amp; Cheese Biscuit Meal</t>
+  </si>
+  <si>
+    <t>6.32</t>
+  </si>
+  <si>
+    <t>Bacon, Egg &amp; Cheese McGriddles Meal</t>
+  </si>
+  <si>
+    <t>570</t>
+  </si>
+  <si>
+    <t>4.49</t>
+  </si>
+  <si>
+    <t>Sausage, Egg &amp; Cheese McGriddles Meal</t>
+  </si>
+  <si>
+    <t>Sausage McGriddles Meal</t>
+  </si>
+  <si>
+    <t>Sausage Burrito Meal</t>
+  </si>
+  <si>
+    <t>4.29</t>
+  </si>
+  <si>
+    <t>Sausage Biscuit</t>
+  </si>
+  <si>
+    <t>460</t>
+  </si>
+  <si>
+    <t>Sausage McMuffin</t>
+  </si>
+  <si>
+    <t>1.19</t>
+  </si>
+  <si>
+    <t>Sausage McGriddles</t>
+  </si>
+  <si>
+    <t>430</t>
+  </si>
+  <si>
+    <t>2.71</t>
+  </si>
+  <si>
+    <t>Hash Browns</t>
+  </si>
+  <si>
+    <t>1.81</t>
+  </si>
+  <si>
+    <t>McDouble</t>
+  </si>
+  <si>
+    <t>3.19</t>
+  </si>
+  <si>
+    <t>3.89</t>
+  </si>
+  <si>
+    <t>Warld Famous Fries</t>
+  </si>
+  <si>
+    <t>230</t>
+  </si>
+  <si>
+    <t>3.79</t>
+  </si>
+  <si>
+    <t>Coca-Cola</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>1.61</t>
+  </si>
+  <si>
+    <t>Sprite</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>Fanta Orange</t>
+  </si>
+  <si>
+    <t>Dr Pepper</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>Bacon, Egg &amp; Cheese Biscuit</t>
+  </si>
+  <si>
+    <t>310</t>
+  </si>
+  <si>
+    <t>1.39</t>
+  </si>
+  <si>
+    <t>Sausage Egg McMuffin</t>
+  </si>
+  <si>
+    <t>480</t>
+  </si>
+  <si>
+    <t>3.39</t>
+  </si>
+  <si>
+    <t>1.79</t>
+  </si>
+  <si>
+    <t>Sausage Egg Biscuit</t>
+  </si>
+  <si>
+    <t>3.69</t>
+  </si>
+  <si>
+    <t>Bacon Egg Cheese McGriddle</t>
+  </si>
+  <si>
+    <t>420</t>
+  </si>
+  <si>
+    <t>3.59</t>
+  </si>
+  <si>
+    <t>Sausage McGriddle</t>
+  </si>
+  <si>
+    <t>2.99</t>
+  </si>
+  <si>
+    <t>Sausage Egg Cheese McGriddle</t>
+  </si>
+  <si>
+    <t>Big Breakfast</t>
+  </si>
+  <si>
+    <t>780</t>
+  </si>
+  <si>
+    <t>4.59</t>
+  </si>
+  <si>
+    <t>Big Breakfast with Hotcakes</t>
+  </si>
+  <si>
+    <t>1340</t>
+  </si>
+  <si>
+    <t>Hotcakes</t>
+  </si>
+  <si>
+    <t>590</t>
+  </si>
+  <si>
+    <t>3.49</t>
+  </si>
+  <si>
+    <t>Hotcakes and Sausage</t>
+  </si>
+  <si>
+    <t>Sausage Burrito</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>1.99</t>
+  </si>
+  <si>
+    <t>2.69</t>
+  </si>
+  <si>
+    <t>Fruit &amp; Maple Oatmeal</t>
+  </si>
+  <si>
+    <t>320</t>
+  </si>
+  <si>
+    <t>World Famous Fries</t>
+  </si>
+  <si>
+    <t>Apple Slices</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>1.20</t>
+  </si>
+  <si>
+    <t>Cheese Danish</t>
+  </si>
+  <si>
+    <t>3.09</t>
+  </si>
+  <si>
+    <t>Apple Fritter</t>
+  </si>
+  <si>
+    <t>510</t>
+  </si>
+  <si>
+    <t>Blueberry Muffin</t>
+  </si>
+  <si>
+    <t>440</t>
+  </si>
+  <si>
+    <t>Cinnamon Roll with Cream Cheese Icing</t>
+  </si>
+  <si>
+    <t>540</t>
+  </si>
+  <si>
+    <t>3.23</t>
+  </si>
+  <si>
+    <t>Caramel Macchiato</t>
+  </si>
+  <si>
+    <t>260</t>
+  </si>
+  <si>
+    <t>Iced Caramel Macchiato</t>
+  </si>
+  <si>
+    <t>210</t>
+  </si>
+  <si>
+    <t>2.40</t>
+  </si>
+  <si>
+    <t>Cappuccino</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>Caramel Cappuccino</t>
+  </si>
+  <si>
+    <t>French Vanilla Cappuccino</t>
+  </si>
+  <si>
+    <t>Mocha</t>
+  </si>
+  <si>
+    <t>360</t>
+  </si>
+  <si>
+    <t>Iced Mocha</t>
+  </si>
+  <si>
+    <t>280</t>
+  </si>
+  <si>
+    <t>2.89</t>
+  </si>
+  <si>
+    <t>Latte</t>
+  </si>
+  <si>
+    <t>Iced Latte</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>Caramel Latte</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>French Vanilla Latte</t>
+  </si>
+  <si>
+    <t>Iced French Vanilla Latte</t>
+  </si>
+  <si>
+    <t>Iced Coffee</t>
+  </si>
+  <si>
+    <t>Iced Caramel Coffee</t>
+  </si>
+  <si>
+    <t>Iced French Vanilla Coffee</t>
+  </si>
+  <si>
+    <t>Caramel FrappÃ©</t>
+  </si>
+  <si>
+    <t>Mocha FrappÃ©</t>
+  </si>
+  <si>
+    <t>Hot Chocolate</t>
+  </si>
+  <si>
+    <t>370</t>
+  </si>
+  <si>
+    <t>Mango Pineapple Smoothie</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>Hamburger Happy Meal</t>
+  </si>
+  <si>
+    <t>475</t>
+  </si>
+  <si>
+    <t>7.19</t>
+  </si>
+  <si>
+    <t>4 Piece Chicken McNuggets</t>
+  </si>
+  <si>
+    <t>225</t>
+  </si>
+  <si>
+    <t>7.29</t>
+  </si>
+  <si>
+    <t>6 Piece Chicken McNuggets</t>
+  </si>
+  <si>
+    <t>3.1</t>
   </si>
 </sst>
 </file>
@@ -867,10 +1521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C158B37-BA23-4696-8C2A-86E31F80181F}">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D167"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="G111" sqref="G111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1734,6 +2388,1482 @@
         <v>64</v>
       </c>
     </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>145</v>
+      </c>
+      <c r="B62" t="s">
+        <v>146</v>
+      </c>
+      <c r="C62" t="s">
+        <v>57</v>
+      </c>
+      <c r="D62" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>145</v>
+      </c>
+      <c r="B63" t="s">
+        <v>148</v>
+      </c>
+      <c r="C63" t="s">
+        <v>149</v>
+      </c>
+      <c r="D63" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>145</v>
+      </c>
+      <c r="B64" t="s">
+        <v>151</v>
+      </c>
+      <c r="C64" t="s">
+        <v>50</v>
+      </c>
+      <c r="D64" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>145</v>
+      </c>
+      <c r="B65" t="s">
+        <v>153</v>
+      </c>
+      <c r="C65" t="s">
+        <v>154</v>
+      </c>
+      <c r="D65" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>145</v>
+      </c>
+      <c r="B66" t="s">
+        <v>156</v>
+      </c>
+      <c r="C66" t="s">
+        <v>157</v>
+      </c>
+      <c r="D66" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>145</v>
+      </c>
+      <c r="B67" t="s">
+        <v>159</v>
+      </c>
+      <c r="C67" t="s">
+        <v>160</v>
+      </c>
+      <c r="D67" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>145</v>
+      </c>
+      <c r="B68" t="s">
+        <v>162</v>
+      </c>
+      <c r="C68" t="s">
+        <v>163</v>
+      </c>
+      <c r="D68" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>145</v>
+      </c>
+      <c r="B69" t="s">
+        <v>165</v>
+      </c>
+      <c r="C69" t="s">
+        <v>166</v>
+      </c>
+      <c r="D69" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>145</v>
+      </c>
+      <c r="B70" t="s">
+        <v>168</v>
+      </c>
+      <c r="C70" t="s">
+        <v>169</v>
+      </c>
+      <c r="D70" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>145</v>
+      </c>
+      <c r="B71" t="s">
+        <v>170</v>
+      </c>
+      <c r="C71" t="s">
+        <v>171</v>
+      </c>
+      <c r="D71" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>145</v>
+      </c>
+      <c r="B72" t="s">
+        <v>173</v>
+      </c>
+      <c r="C72" t="s">
+        <v>26</v>
+      </c>
+      <c r="D72" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>145</v>
+      </c>
+      <c r="B73" t="s">
+        <v>175</v>
+      </c>
+      <c r="C73" t="s">
+        <v>169</v>
+      </c>
+      <c r="D73" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>145</v>
+      </c>
+      <c r="B74" t="s">
+        <v>177</v>
+      </c>
+      <c r="C74" t="s">
+        <v>178</v>
+      </c>
+      <c r="D74" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>145</v>
+      </c>
+      <c r="B75" t="s">
+        <v>180</v>
+      </c>
+      <c r="C75" t="s">
+        <v>181</v>
+      </c>
+      <c r="D75" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>145</v>
+      </c>
+      <c r="B76" t="s">
+        <v>183</v>
+      </c>
+      <c r="C76" t="s">
+        <v>184</v>
+      </c>
+      <c r="D76" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>145</v>
+      </c>
+      <c r="B77" t="s">
+        <v>185</v>
+      </c>
+      <c r="C77" t="s">
+        <v>186</v>
+      </c>
+      <c r="D77" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>145</v>
+      </c>
+      <c r="B78" t="s">
+        <v>188</v>
+      </c>
+      <c r="C78" t="s">
+        <v>63</v>
+      </c>
+      <c r="D78" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>145</v>
+      </c>
+      <c r="B79" t="s">
+        <v>190</v>
+      </c>
+      <c r="C79" t="s">
+        <v>72</v>
+      </c>
+      <c r="D79" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>145</v>
+      </c>
+      <c r="B80" t="s">
+        <v>192</v>
+      </c>
+      <c r="C80" t="s">
+        <v>193</v>
+      </c>
+      <c r="D80" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>145</v>
+      </c>
+      <c r="B81" t="s">
+        <v>195</v>
+      </c>
+      <c r="C81" t="s">
+        <v>15</v>
+      </c>
+      <c r="D81" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>145</v>
+      </c>
+      <c r="B82" t="s">
+        <v>197</v>
+      </c>
+      <c r="C82" t="s">
+        <v>37</v>
+      </c>
+      <c r="D82" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>145</v>
+      </c>
+      <c r="B83" t="s">
+        <v>198</v>
+      </c>
+      <c r="C83" t="s">
+        <v>84</v>
+      </c>
+      <c r="D83" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>145</v>
+      </c>
+      <c r="B84" t="s">
+        <v>200</v>
+      </c>
+      <c r="C84" t="s">
+        <v>201</v>
+      </c>
+      <c r="D84" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>145</v>
+      </c>
+      <c r="B85" t="s">
+        <v>202</v>
+      </c>
+      <c r="C85" t="s">
+        <v>149</v>
+      </c>
+      <c r="D85" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>145</v>
+      </c>
+      <c r="B86" t="s">
+        <v>204</v>
+      </c>
+      <c r="C86" t="s">
+        <v>69</v>
+      </c>
+      <c r="D86" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>145</v>
+      </c>
+      <c r="B87" t="s">
+        <v>205</v>
+      </c>
+      <c r="C87" t="s">
+        <v>169</v>
+      </c>
+      <c r="D87" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>145</v>
+      </c>
+      <c r="B88" t="s">
+        <v>206</v>
+      </c>
+      <c r="C88" t="s">
+        <v>181</v>
+      </c>
+      <c r="D88" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>207</v>
+      </c>
+      <c r="B89" t="s">
+        <v>208</v>
+      </c>
+      <c r="C89" t="s">
+        <v>209</v>
+      </c>
+      <c r="D89" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>207</v>
+      </c>
+      <c r="B90" t="s">
+        <v>211</v>
+      </c>
+      <c r="C90" t="s">
+        <v>212</v>
+      </c>
+      <c r="D90" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>207</v>
+      </c>
+      <c r="B91" t="s">
+        <v>214</v>
+      </c>
+      <c r="C91" t="s">
+        <v>209</v>
+      </c>
+      <c r="D91" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>207</v>
+      </c>
+      <c r="B92" t="s">
+        <v>215</v>
+      </c>
+      <c r="C92" t="s">
+        <v>209</v>
+      </c>
+      <c r="D92" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>207</v>
+      </c>
+      <c r="B93" t="s">
+        <v>216</v>
+      </c>
+      <c r="C93" t="s">
+        <v>217</v>
+      </c>
+      <c r="D93" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>207</v>
+      </c>
+      <c r="B94" t="s">
+        <v>218</v>
+      </c>
+      <c r="C94" t="s">
+        <v>219</v>
+      </c>
+      <c r="D94" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>207</v>
+      </c>
+      <c r="B95" t="s">
+        <v>220</v>
+      </c>
+      <c r="C95" t="s">
+        <v>178</v>
+      </c>
+      <c r="D95" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>207</v>
+      </c>
+      <c r="B96" t="s">
+        <v>222</v>
+      </c>
+      <c r="C96" t="s">
+        <v>54</v>
+      </c>
+      <c r="D96" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>207</v>
+      </c>
+      <c r="B97" t="s">
+        <v>223</v>
+      </c>
+      <c r="C97" t="s">
+        <v>224</v>
+      </c>
+      <c r="D97" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>207</v>
+      </c>
+      <c r="B98" t="s">
+        <v>225</v>
+      </c>
+      <c r="C98" t="s">
+        <v>72</v>
+      </c>
+      <c r="D98" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>207</v>
+      </c>
+      <c r="B99" t="s">
+        <v>227</v>
+      </c>
+      <c r="C99" t="s">
+        <v>228</v>
+      </c>
+      <c r="D99" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>207</v>
+      </c>
+      <c r="B100" t="s">
+        <v>230</v>
+      </c>
+      <c r="C100" t="s">
+        <v>16</v>
+      </c>
+      <c r="D100" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>207</v>
+      </c>
+      <c r="B101" t="s">
+        <v>232</v>
+      </c>
+      <c r="C101" t="s">
+        <v>63</v>
+      </c>
+      <c r="D101" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>207</v>
+      </c>
+      <c r="B102" t="s">
+        <v>233</v>
+      </c>
+      <c r="C102" t="s">
+        <v>209</v>
+      </c>
+      <c r="D102" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>207</v>
+      </c>
+      <c r="B103" t="s">
+        <v>234</v>
+      </c>
+      <c r="C103" t="s">
+        <v>235</v>
+      </c>
+      <c r="D103" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>207</v>
+      </c>
+      <c r="B104" t="s">
+        <v>237</v>
+      </c>
+      <c r="C104" t="s">
+        <v>31</v>
+      </c>
+      <c r="D104" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>207</v>
+      </c>
+      <c r="B105" t="s">
+        <v>239</v>
+      </c>
+      <c r="C105" t="s">
+        <v>240</v>
+      </c>
+      <c r="D105" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>207</v>
+      </c>
+      <c r="B106" t="s">
+        <v>241</v>
+      </c>
+      <c r="C106" t="s">
+        <v>18</v>
+      </c>
+      <c r="D106" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>207</v>
+      </c>
+      <c r="B107" t="s">
+        <v>243</v>
+      </c>
+      <c r="C107" t="s">
+        <v>244</v>
+      </c>
+      <c r="D107" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>207</v>
+      </c>
+      <c r="B108" t="s">
+        <v>246</v>
+      </c>
+      <c r="C108" t="s">
+        <v>169</v>
+      </c>
+      <c r="D108" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>207</v>
+      </c>
+      <c r="B109" t="s">
+        <v>247</v>
+      </c>
+      <c r="C109" t="s">
+        <v>244</v>
+      </c>
+      <c r="D109" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>207</v>
+      </c>
+      <c r="B110" t="s">
+        <v>248</v>
+      </c>
+      <c r="C110" t="s">
+        <v>235</v>
+      </c>
+      <c r="D110" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>207</v>
+      </c>
+      <c r="B111" t="s">
+        <v>250</v>
+      </c>
+      <c r="C111" t="s">
+        <v>251</v>
+      </c>
+      <c r="D111" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>207</v>
+      </c>
+      <c r="B112" t="s">
+        <v>252</v>
+      </c>
+      <c r="C112" t="s">
+        <v>219</v>
+      </c>
+      <c r="D112" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>207</v>
+      </c>
+      <c r="B113" t="s">
+        <v>254</v>
+      </c>
+      <c r="C113" t="s">
+        <v>255</v>
+      </c>
+      <c r="D113" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>207</v>
+      </c>
+      <c r="B114" t="s">
+        <v>257</v>
+      </c>
+      <c r="C114" t="s">
+        <v>255</v>
+      </c>
+      <c r="D114" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>207</v>
+      </c>
+      <c r="B115" t="s">
+        <v>259</v>
+      </c>
+      <c r="C115" t="s">
+        <v>219</v>
+      </c>
+      <c r="D115" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>207</v>
+      </c>
+      <c r="B116" t="s">
+        <v>218</v>
+      </c>
+      <c r="C116" t="s">
+        <v>219</v>
+      </c>
+      <c r="D116" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>207</v>
+      </c>
+      <c r="B117" t="s">
+        <v>216</v>
+      </c>
+      <c r="C117" t="s">
+        <v>217</v>
+      </c>
+      <c r="D117" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>207</v>
+      </c>
+      <c r="B118" t="s">
+        <v>262</v>
+      </c>
+      <c r="C118" t="s">
+        <v>263</v>
+      </c>
+      <c r="D118" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>207</v>
+      </c>
+      <c r="B119" t="s">
+        <v>265</v>
+      </c>
+      <c r="C119" t="s">
+        <v>266</v>
+      </c>
+      <c r="D119" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>207</v>
+      </c>
+      <c r="B120" t="s">
+        <v>268</v>
+      </c>
+      <c r="C120" t="s">
+        <v>269</v>
+      </c>
+      <c r="D120" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>207</v>
+      </c>
+      <c r="B121" t="s">
+        <v>270</v>
+      </c>
+      <c r="C121" t="s">
+        <v>266</v>
+      </c>
+      <c r="D121" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>207</v>
+      </c>
+      <c r="B122" t="s">
+        <v>271</v>
+      </c>
+      <c r="C122" t="s">
+        <v>272</v>
+      </c>
+      <c r="D122" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>207</v>
+      </c>
+      <c r="B123" t="s">
+        <v>273</v>
+      </c>
+      <c r="C123" t="s">
+        <v>235</v>
+      </c>
+      <c r="D123" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>207</v>
+      </c>
+      <c r="B124" t="s">
+        <v>234</v>
+      </c>
+      <c r="C124" t="s">
+        <v>274</v>
+      </c>
+      <c r="D124" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>207</v>
+      </c>
+      <c r="B125" t="s">
+        <v>252</v>
+      </c>
+      <c r="C125" t="s">
+        <v>219</v>
+      </c>
+      <c r="D125" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>207</v>
+      </c>
+      <c r="B126" t="s">
+        <v>276</v>
+      </c>
+      <c r="C126" t="s">
+        <v>277</v>
+      </c>
+      <c r="D126" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>207</v>
+      </c>
+      <c r="B127" t="s">
+        <v>250</v>
+      </c>
+      <c r="C127" t="s">
+        <v>251</v>
+      </c>
+      <c r="D127" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>207</v>
+      </c>
+      <c r="B128" t="s">
+        <v>280</v>
+      </c>
+      <c r="C128" t="s">
+        <v>209</v>
+      </c>
+      <c r="D128" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>207</v>
+      </c>
+      <c r="B129" t="s">
+        <v>282</v>
+      </c>
+      <c r="C129" t="s">
+        <v>283</v>
+      </c>
+      <c r="D129" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>207</v>
+      </c>
+      <c r="B130" t="s">
+        <v>285</v>
+      </c>
+      <c r="C130" t="s">
+        <v>255</v>
+      </c>
+      <c r="D130" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>207</v>
+      </c>
+      <c r="B131" t="s">
+        <v>287</v>
+      </c>
+      <c r="C131" t="s">
+        <v>33</v>
+      </c>
+      <c r="D131" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>207</v>
+      </c>
+      <c r="B132" t="s">
+        <v>288</v>
+      </c>
+      <c r="C132" t="s">
+        <v>289</v>
+      </c>
+      <c r="D132" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>207</v>
+      </c>
+      <c r="B133" t="s">
+        <v>291</v>
+      </c>
+      <c r="C133" t="s">
+        <v>292</v>
+      </c>
+      <c r="D133" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>207</v>
+      </c>
+      <c r="B134" t="s">
+        <v>293</v>
+      </c>
+      <c r="C134" t="s">
+        <v>294</v>
+      </c>
+      <c r="D134" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>207</v>
+      </c>
+      <c r="B135" t="s">
+        <v>296</v>
+      </c>
+      <c r="C135" t="s">
+        <v>289</v>
+      </c>
+      <c r="D135" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>207</v>
+      </c>
+      <c r="B136" t="s">
+        <v>297</v>
+      </c>
+      <c r="C136" t="s">
+        <v>298</v>
+      </c>
+      <c r="D136" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>207</v>
+      </c>
+      <c r="B137" t="s">
+        <v>257</v>
+      </c>
+      <c r="C137" t="s">
+        <v>266</v>
+      </c>
+      <c r="D137" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>207</v>
+      </c>
+      <c r="B138" t="s">
+        <v>301</v>
+      </c>
+      <c r="C138" t="s">
+        <v>302</v>
+      </c>
+      <c r="D138" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>207</v>
+      </c>
+      <c r="B139" t="s">
+        <v>303</v>
+      </c>
+      <c r="C139" t="s">
+        <v>263</v>
+      </c>
+      <c r="D139" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>207</v>
+      </c>
+      <c r="B140" t="s">
+        <v>304</v>
+      </c>
+      <c r="C140" t="s">
+        <v>305</v>
+      </c>
+      <c r="D140" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>207</v>
+      </c>
+      <c r="B141" t="s">
+        <v>307</v>
+      </c>
+      <c r="C141" t="s">
+        <v>178</v>
+      </c>
+      <c r="D141" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>207</v>
+      </c>
+      <c r="B142" t="s">
+        <v>309</v>
+      </c>
+      <c r="C142" t="s">
+        <v>310</v>
+      </c>
+      <c r="D142" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>207</v>
+      </c>
+      <c r="B143" t="s">
+        <v>311</v>
+      </c>
+      <c r="C143" t="s">
+        <v>312</v>
+      </c>
+      <c r="D143" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>207</v>
+      </c>
+      <c r="B144" t="s">
+        <v>313</v>
+      </c>
+      <c r="C144" t="s">
+        <v>314</v>
+      </c>
+      <c r="D144" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>207</v>
+      </c>
+      <c r="B145" t="s">
+        <v>316</v>
+      </c>
+      <c r="C145" t="s">
+        <v>317</v>
+      </c>
+      <c r="D145" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>207</v>
+      </c>
+      <c r="B146" t="s">
+        <v>318</v>
+      </c>
+      <c r="C146" t="s">
+        <v>319</v>
+      </c>
+      <c r="D146" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>207</v>
+      </c>
+      <c r="B147" t="s">
+        <v>321</v>
+      </c>
+      <c r="C147" t="s">
+        <v>322</v>
+      </c>
+      <c r="D147" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>207</v>
+      </c>
+      <c r="B148" t="s">
+        <v>323</v>
+      </c>
+      <c r="C148" t="s">
+        <v>319</v>
+      </c>
+      <c r="D148" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>207</v>
+      </c>
+      <c r="B149" t="s">
+        <v>324</v>
+      </c>
+      <c r="C149" t="s">
+        <v>319</v>
+      </c>
+      <c r="D149" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>207</v>
+      </c>
+      <c r="B150" t="s">
+        <v>325</v>
+      </c>
+      <c r="C150" t="s">
+        <v>326</v>
+      </c>
+      <c r="D150" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>207</v>
+      </c>
+      <c r="B151" t="s">
+        <v>327</v>
+      </c>
+      <c r="C151" t="s">
+        <v>328</v>
+      </c>
+      <c r="D151" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>207</v>
+      </c>
+      <c r="B152" t="s">
+        <v>330</v>
+      </c>
+      <c r="C152" t="s">
+        <v>269</v>
+      </c>
+      <c r="D152" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>207</v>
+      </c>
+      <c r="B153" t="s">
+        <v>331</v>
+      </c>
+      <c r="C153" t="s">
+        <v>332</v>
+      </c>
+      <c r="D153" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>207</v>
+      </c>
+      <c r="B154" t="s">
+        <v>333</v>
+      </c>
+      <c r="C154" t="s">
+        <v>334</v>
+      </c>
+      <c r="D154" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>207</v>
+      </c>
+      <c r="B155" t="s">
+        <v>335</v>
+      </c>
+      <c r="C155" t="s">
+        <v>334</v>
+      </c>
+      <c r="D155" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>207</v>
+      </c>
+      <c r="B156" t="s">
+        <v>336</v>
+      </c>
+      <c r="C156" t="s">
+        <v>319</v>
+      </c>
+      <c r="D156" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>207</v>
+      </c>
+      <c r="B157" t="s">
+        <v>337</v>
+      </c>
+      <c r="C157" t="s">
+        <v>269</v>
+      </c>
+      <c r="D157" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>207</v>
+      </c>
+      <c r="B158" t="s">
+        <v>338</v>
+      </c>
+      <c r="C158" t="s">
+        <v>269</v>
+      </c>
+      <c r="D158" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>207</v>
+      </c>
+      <c r="B159" t="s">
+        <v>339</v>
+      </c>
+      <c r="C159" t="s">
+        <v>322</v>
+      </c>
+      <c r="D159" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>207</v>
+      </c>
+      <c r="B160" t="s">
+        <v>340</v>
+      </c>
+      <c r="C160" t="s">
+        <v>255</v>
+      </c>
+      <c r="D160" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>207</v>
+      </c>
+      <c r="B161" t="s">
+        <v>341</v>
+      </c>
+      <c r="C161" t="s">
+        <v>283</v>
+      </c>
+      <c r="D161" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>207</v>
+      </c>
+      <c r="B162" t="s">
+        <v>342</v>
+      </c>
+      <c r="C162" t="s">
+        <v>343</v>
+      </c>
+      <c r="D162" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>207</v>
+      </c>
+      <c r="B163" t="s">
+        <v>344</v>
+      </c>
+      <c r="C163" t="s">
+        <v>345</v>
+      </c>
+      <c r="D163" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>207</v>
+      </c>
+      <c r="B164" t="s">
+        <v>346</v>
+      </c>
+      <c r="C164" t="s">
+        <v>347</v>
+      </c>
+      <c r="D164" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>207</v>
+      </c>
+      <c r="B165" t="s">
+        <v>349</v>
+      </c>
+      <c r="C165" t="s">
+        <v>350</v>
+      </c>
+      <c r="D165" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>207</v>
+      </c>
+      <c r="B166" t="s">
+        <v>352</v>
+      </c>
+      <c r="C166" t="s">
+        <v>347</v>
+      </c>
+      <c r="D166" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167"/>
+      <c r="B167"/>
+      <c r="C167"/>
+      <c r="D167"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>